<commit_message>
updated list of outputs
</commit_message>
<xml_diff>
--- a/docs/_static/INSaFLU_current_outputs_25_03_2021.xlsx
+++ b/docs/_static/INSaFLU_current_outputs_25_03_2021.xlsx
@@ -1219,21 +1219,107 @@
   </si>
   <si>
     <r>
-      <t>Consensus amino acid alignments per encoded protein.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> NOTE: sequences are exclusively generated for locus with 100% of its length covered by ≥X-fold)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Projects / Show project results /</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Amino acid alignments by MSAViewer</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">A version of the reference sequence with all validated variants replaced and undefined nucleotides (NNN) placed in low coverage regions (i.e., regions with coverage below </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">). NOTE: consensus sequences are exclusively generated for locus with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>% of its length covered by ≥</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-fold) (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GREEN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1242,13 +1328,97 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YELLOW</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
         <b/>
         <sz val="9"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">(X = mincov; user-defined setting)  </t>
+      <t xml:space="preserve">(X = mincov; Y = minimum horizontal coverage; user-defined settings) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>#</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Compiles the coverage reports for each sample, including the following data: mean depth of coverage </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">per </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">locus, % of locus size covered by at least 1-fold and % of locus size covered by at least X-fold. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(X = mincov; user-defined setting)</t>
     </r>
     <r>
       <rPr>
@@ -1259,97 +1429,10 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>#</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Projects / Show project results /</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Amino acid alignments by MSAViewer</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">A version of the reference sequence with all validated variants replaced and undefined nucleotides (NNN) placed in low coverage regions (i.e., regions with coverage below </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">). NOTE: consensus sequences are exclusively generated for locus with </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Y</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>% of its length covered by ≥</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-fold) (</t>
-    </r>
+      <t xml:space="preserve">  #</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -1359,10 +1442,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>GREEN</t>
-    </r>
-    <r>
-      <rPr>
+      <t>GREEN:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="12"/>
         <color rgb="FF00B0F0"/>
         <rFont val="Calibri"/>
@@ -1373,42 +1457,13 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>and</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>YELLOW</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>% of locus size covered by at least X-fold = 100%</t>
     </r>
     <r>
       <rPr>
@@ -1418,52 +1473,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">(X = mincov; Y = minimum horizontal coverage; user-defined settings) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>#</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Compiles the coverage reports for each sample, including the following data: mean depth of coverage </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">per </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">locus, % of locus size covered by at least 1-fold and % of locus size covered by at least X-fold. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(X = mincov; user-defined setting)</t>
+      <t xml:space="preserve"> (X = mincov; user-defined setting)  </t>
     </r>
     <r>
       <rPr>
@@ -1474,26 +1484,26 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">  #</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>GREEN:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF00B0F0"/>
+      <t>#</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YELLOW:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1508,7 +1518,35 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>% of locus size covered by at least X-fold = 100%</t>
+      <t xml:space="preserve">% of locus size covered by at least X-fold is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>≥</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Y% and &lt; 100%.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -1518,7 +1556,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (X = mincov; user-defined setting)  </t>
+      <t>(X = mincov; Y = minimum horizontal coverage; user-defined settings)</t>
     </r>
     <r>
       <rPr>
@@ -1529,10 +1567,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>#</t>
-    </r>
-  </si>
-  <si>
+      <t xml:space="preserve"> #</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RED:</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -1542,17 +1591,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>YELLOW:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve"> </t>
     </r>
     <r>
@@ -1563,30 +1601,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">% of locus size covered by at least X-fold is </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>≥</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Y% and &lt; 100%.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
+      <t>% of locus size covered by at least X-fold is &lt;Y%</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1617,71 +1637,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>RED:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>% of locus size covered by at least X-fold is &lt;Y%</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(X = mincov; Y = minimum horizontal coverage; user-defined settings)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> #</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">* Consensus sequences are exclusively generated for locus with Y% of its length covered by ≥X-fold) (X = mincov; Y = minimum horizontal coverage; user-defined settings) </t>
     </r>
     <r>
@@ -2233,6 +2188,21 @@
   </si>
   <si>
     <t>last update to the file: 25 March 2021</t>
+  </si>
+  <si>
+    <r>
+      <t>Consensus amino acid alignments per encoded protein.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> NOTE: protein alignments only include samples with &lt;10% of undefined amino acids (X).</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2862,6 +2832,15 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2899,15 +2878,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3277,7 +3247,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -3306,7 +3276,7 @@
     </row>
     <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="66" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -3318,7 +3288,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>16</v>
@@ -3334,30 +3304,30 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="70" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="61" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="68"/>
+      <c r="A6" s="71"/>
       <c r="B6" s="57"/>
       <c r="C6" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D6" s="27" t="s">
         <v>6</v>
@@ -3370,10 +3340,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="68"/>
+      <c r="A7" s="71"/>
       <c r="B7" s="63"/>
       <c r="C7" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D7" s="27" t="s">
         <v>5</v>
@@ -3390,7 +3360,7 @@
         <v>59</v>
       </c>
       <c r="B8" s="62" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" s="45" t="s">
         <v>62</v>
@@ -3452,11 +3422,11 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="71" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="64" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>8</v>
@@ -3472,7 +3442,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="68"/>
+      <c r="A13" s="71"/>
       <c r="B13" s="64"/>
       <c r="C13" s="18" t="s">
         <v>10</v>
@@ -3488,7 +3458,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="68"/>
+      <c r="A14" s="71"/>
       <c r="B14" s="57"/>
       <c r="C14" s="20" t="s">
         <v>29</v>
@@ -3504,7 +3474,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="68"/>
+      <c r="A15" s="71"/>
       <c r="B15" s="57"/>
       <c r="C15" s="20" t="s">
         <v>30</v>
@@ -3520,7 +3490,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="68"/>
+      <c r="A16" s="71"/>
       <c r="B16" s="57"/>
       <c r="C16" s="21" t="s">
         <v>40</v>
@@ -3529,7 +3499,7 @@
         <v>13</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F16" s="41" t="s">
         <v>72</v>
@@ -3540,7 +3510,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="65" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>31</v>
@@ -3549,7 +3519,7 @@
         <v>14</v>
       </c>
       <c r="E17" s="48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>57</v>
@@ -3558,38 +3528,38 @@
     <row r="18" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
-      <c r="C18" s="77" t="s">
+      <c r="C18" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="74" t="s">
+      <c r="D18" s="77" t="s">
         <v>18</v>
       </c>
       <c r="E18" s="51" t="s">
-        <v>80</v>
-      </c>
-      <c r="F18" s="71" t="s">
-        <v>98</v>
+        <v>79</v>
+      </c>
+      <c r="F18" s="74" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
-      <c r="C19" s="78"/>
-      <c r="D19" s="75"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="78"/>
       <c r="E19" s="52" t="s">
-        <v>81</v>
-      </c>
-      <c r="F19" s="72"/>
+        <v>80</v>
+      </c>
+      <c r="F19" s="75"/>
     </row>
     <row r="20" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
-      <c r="C20" s="79"/>
-      <c r="D20" s="76"/>
+      <c r="C20" s="82"/>
+      <c r="D20" s="79"/>
       <c r="E20" s="53" t="s">
-        <v>82</v>
-      </c>
-      <c r="F20" s="73"/>
+        <v>81</v>
+      </c>
+      <c r="F20" s="76"/>
     </row>
     <row r="21" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
@@ -3624,7 +3594,7 @@
         <v>3</v>
       </c>
       <c r="B23" s="64" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>39</v>
@@ -3633,13 +3603,13 @@
         <v>20</v>
       </c>
       <c r="E23" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F23" s="50" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="96.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="20" t="s">
@@ -3649,7 +3619,7 @@
         <v>20</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F24" s="50" t="s">
         <v>75</v>
@@ -3665,10 +3635,10 @@
         <v>20</v>
       </c>
       <c r="E25" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" s="50" t="s">
         <v>76</v>
-      </c>
-      <c r="F25" s="50" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3681,7 +3651,7 @@
         <v>23</v>
       </c>
       <c r="E26" s="34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>67</v>
@@ -3697,53 +3667,53 @@
         <v>23</v>
       </c>
       <c r="E27" s="34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="129" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="69" t="s">
+      <c r="A28" s="72" t="s">
         <v>4</v>
       </c>
       <c r="B28" s="62" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D28" s="28" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F28" s="54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="36" customFormat="1" ht="87.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="69"/>
+      <c r="A29" s="72"/>
       <c r="B29" s="58"/>
       <c r="C29" s="37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D29" s="28" t="s">
         <v>14</v>
       </c>
       <c r="E29" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F29" s="55" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="193.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="70"/>
+      <c r="A30" s="73"/>
       <c r="B30" s="59"/>
       <c r="C30" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D30" s="60" t="s">
         <v>18</v>
@@ -3758,7 +3728,7 @@
         <v>25</v>
       </c>
       <c r="B31" s="64" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C31" s="18" t="s">
         <v>35</v>
@@ -3767,51 +3737,51 @@
         <v>28</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="82" t="s">
-        <v>83</v>
-      </c>
-      <c r="B32" s="82"/>
-      <c r="C32" s="82"/>
-      <c r="D32" s="82"/>
-      <c r="E32" s="82"/>
+      <c r="A32" s="69" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="69"/>
+      <c r="C32" s="69"/>
+      <c r="D32" s="69"/>
+      <c r="E32" s="69"/>
       <c r="F32" s="6"/>
     </row>
     <row r="33" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="80" t="s">
-        <v>84</v>
-      </c>
-      <c r="B33" s="80"/>
-      <c r="C33" s="80"/>
-      <c r="D33" s="80"/>
-      <c r="E33" s="80"/>
+      <c r="A33" s="67" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="67"/>
+      <c r="C33" s="67"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="67"/>
     </row>
     <row r="34" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="81" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" s="81"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="81"/>
-      <c r="E34" s="81"/>
+      <c r="A34" s="68" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="68"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="C18:C20"/>
     <mergeCell ref="A33:E33"/>
     <mergeCell ref="A34:E34"/>
     <mergeCell ref="A32:E32"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="A28:A30"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="C18:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>